<commit_message>
TEST: Add forecast tests
</commit_message>
<xml_diff>
--- a/autodcf/tests/data/simple_dcf.xlsx
+++ b/autodcf/tests/data/simple_dcf.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacklm/Documents/Interests/Programming/Python/autodcf/autodcf/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60967A96-8F9C-4447-91C8-5C8A56508E51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14122429-D573-2448-9648-1C3253AA0FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{F59C2343-CAF4-9248-9F9B-A15401A49AE8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="2" xr2:uid="{F59C2343-CAF4-9248-9F9B-A15401A49AE8}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="1" r:id="rId1"/>
     <sheet name="Assumptions" sheetId="2" r:id="rId2"/>
+    <sheet name="Results" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -100,18 +101,6 @@
     <t>Tax Rate</t>
   </si>
   <si>
-    <t>Net Debt</t>
-  </si>
-  <si>
-    <t>Discounted Cash Flows</t>
-  </si>
-  <si>
-    <t>Discounted Terminal Cash Flow</t>
-  </si>
-  <si>
-    <t>DCF</t>
-  </si>
-  <si>
     <t>Terminal Growth Rate</t>
   </si>
   <si>
@@ -119,6 +108,33 @@
   </si>
   <si>
     <t>Today's Date</t>
+  </si>
+  <si>
+    <t>discounted_window_cash_flow</t>
+  </si>
+  <si>
+    <t>discounted_terminal_cash_flow</t>
+  </si>
+  <si>
+    <t>net_debt</t>
+  </si>
+  <si>
+    <t>equity_value</t>
+  </si>
+  <si>
+    <t>fully_diluted_shares</t>
+  </si>
+  <si>
+    <t>equity_value_per_share</t>
+  </si>
+  <si>
+    <t>enterprise_value</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -128,7 +144,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -175,14 +191,16 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -501,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE14D32-AA9A-A74F-9608-31C4FBD86A23}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -599,21 +617,21 @@
         <v>50</v>
       </c>
       <c r="E2" s="4">
-        <f>C2-D2</f>
+        <f t="shared" ref="E2:E8" si="0">C2-D2</f>
         <v>50</v>
       </c>
       <c r="F2" s="4">
         <v>25</v>
       </c>
       <c r="G2" s="4">
-        <f>E2-F2</f>
+        <f t="shared" ref="G2:G8" si="1">E2-F2</f>
         <v>25</v>
       </c>
       <c r="H2" s="4">
         <v>2</v>
       </c>
       <c r="I2" s="4">
-        <f>G2-H2</f>
+        <f t="shared" ref="I2:I8" si="2">G2-H2</f>
         <v>23</v>
       </c>
       <c r="J2" s="4">
@@ -621,21 +639,21 @@
         <v>6</v>
       </c>
       <c r="K2" s="4">
-        <f>I2-J2</f>
+        <f t="shared" ref="K2:K8" si="3">I2-J2</f>
         <v>17</v>
       </c>
       <c r="L2" s="4">
         <v>1</v>
       </c>
       <c r="M2" s="4">
-        <f>K2-L2</f>
+        <f t="shared" ref="M2:M8" si="4">K2-L2</f>
         <v>16</v>
       </c>
       <c r="N2" s="4">
         <v>4</v>
       </c>
       <c r="O2" s="4">
-        <f>M2-N2</f>
+        <f t="shared" ref="O2:O8" si="5">M2-N2</f>
         <v>12</v>
       </c>
       <c r="P2" s="4">
@@ -645,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="4">
-        <f>O2+J2-P2-Q2</f>
+        <f t="shared" ref="R2:R8" si="6">O2+J2-P2-Q2</f>
         <v>15</v>
       </c>
       <c r="S2" s="4"/>
@@ -655,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <f ca="1">B2+1</f>
+        <f t="shared" ref="B3:B8" ca="1" si="7">B2+1</f>
         <v>2020</v>
       </c>
       <c r="C3" s="4">
@@ -667,7 +685,7 @@
         <v>51.5</v>
       </c>
       <c r="E3" s="4">
-        <f>C3-D3</f>
+        <f t="shared" si="0"/>
         <v>51.5</v>
       </c>
       <c r="F3" s="4">
@@ -675,7 +693,7 @@
         <v>25.75</v>
       </c>
       <c r="G3" s="4">
-        <f>E3-F3</f>
+        <f t="shared" si="1"/>
         <v>25.75</v>
       </c>
       <c r="H3" s="4">
@@ -683,7 +701,7 @@
         <v>2.06</v>
       </c>
       <c r="I3" s="4">
-        <f>G3-H3</f>
+        <f t="shared" si="2"/>
         <v>23.69</v>
       </c>
       <c r="J3" s="4">
@@ -691,7 +709,7 @@
         <v>6.18</v>
       </c>
       <c r="K3" s="4">
-        <f>I3-J3</f>
+        <f t="shared" si="3"/>
         <v>17.510000000000002</v>
       </c>
       <c r="L3" s="4">
@@ -699,7 +717,7 @@
         <v>1.03</v>
       </c>
       <c r="M3" s="4">
-        <f>K3-L3</f>
+        <f t="shared" si="4"/>
         <v>16.48</v>
       </c>
       <c r="N3" s="4">
@@ -707,7 +725,7 @@
         <v>3.4607999999999999</v>
       </c>
       <c r="O3" s="4">
-        <f>M3-N3</f>
+        <f t="shared" si="5"/>
         <v>13.019200000000001</v>
       </c>
       <c r="P3" s="4">
@@ -719,7 +737,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="R3" s="4">
-        <f>O3+J3-P3-Q3</f>
+        <f t="shared" si="6"/>
         <v>15.809200000000001</v>
       </c>
       <c r="S3" s="4">
@@ -733,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">B3+1</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
       <c r="C4" s="4">
@@ -745,7 +763,7 @@
         <v>53.045000000000002</v>
       </c>
       <c r="E4" s="4">
-        <f>C4-D4</f>
+        <f t="shared" si="0"/>
         <v>53.045000000000002</v>
       </c>
       <c r="F4" s="4">
@@ -753,7 +771,7 @@
         <v>26.522500000000001</v>
       </c>
       <c r="G4" s="4">
-        <f>E4-F4</f>
+        <f t="shared" si="1"/>
         <v>26.522500000000001</v>
       </c>
       <c r="H4" s="4">
@@ -761,7 +779,7 @@
         <v>2.1217999999999999</v>
       </c>
       <c r="I4" s="4">
-        <f>G4-H4</f>
+        <f t="shared" si="2"/>
         <v>24.400700000000001</v>
       </c>
       <c r="J4" s="4">
@@ -769,7 +787,7 @@
         <v>6.3654000000000002</v>
       </c>
       <c r="K4" s="4">
-        <f>I4-J4</f>
+        <f t="shared" si="3"/>
         <v>18.035299999999999</v>
       </c>
       <c r="L4" s="4">
@@ -777,7 +795,7 @@
         <v>1.0609</v>
       </c>
       <c r="M4" s="4">
-        <f>K4-L4</f>
+        <f t="shared" si="4"/>
         <v>16.974399999999999</v>
       </c>
       <c r="N4" s="4">
@@ -785,7 +803,7 @@
         <v>3.5646239999999998</v>
       </c>
       <c r="O4" s="4">
-        <f>M4-N4</f>
+        <f t="shared" si="5"/>
         <v>13.409775999999999</v>
       </c>
       <c r="P4" s="4">
@@ -797,7 +815,7 @@
         <v>0.30900000000000039</v>
       </c>
       <c r="R4" s="4">
-        <f>O4+J4-P4-Q4</f>
+        <f t="shared" si="6"/>
         <v>16.283475999999997</v>
       </c>
       <c r="S4" s="4">
@@ -811,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <f ca="1">B4+1</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2022</v>
       </c>
       <c r="C5" s="4">
@@ -823,7 +841,7 @@
         <v>54.63635</v>
       </c>
       <c r="E5" s="4">
-        <f>C5-D5</f>
+        <f t="shared" si="0"/>
         <v>54.63635</v>
       </c>
       <c r="F5" s="4">
@@ -831,7 +849,7 @@
         <v>27.318175</v>
       </c>
       <c r="G5" s="4">
-        <f>E5-F5</f>
+        <f t="shared" si="1"/>
         <v>27.318175</v>
       </c>
       <c r="H5" s="4">
@@ -839,7 +857,7 @@
         <v>2.185454</v>
       </c>
       <c r="I5" s="4">
-        <f>G5-H5</f>
+        <f t="shared" si="2"/>
         <v>25.132721</v>
       </c>
       <c r="J5" s="4">
@@ -847,7 +865,7 @@
         <v>6.556362</v>
       </c>
       <c r="K5" s="4">
-        <f>I5-J5</f>
+        <f t="shared" si="3"/>
         <v>18.576359</v>
       </c>
       <c r="L5" s="4">
@@ -855,7 +873,7 @@
         <v>1.092727</v>
       </c>
       <c r="M5" s="4">
-        <f>K5-L5</f>
+        <f t="shared" si="4"/>
         <v>17.483632</v>
       </c>
       <c r="N5" s="4">
@@ -863,7 +881,7 @@
         <v>3.6715627199999998</v>
       </c>
       <c r="O5" s="4">
-        <f>M5-N5</f>
+        <f t="shared" si="5"/>
         <v>13.812069279999999</v>
       </c>
       <c r="P5" s="4">
@@ -875,7 +893,7 @@
         <v>0.31826999999999972</v>
       </c>
       <c r="R5" s="4">
-        <f>O5+J5-P5-Q5</f>
+        <f t="shared" si="6"/>
         <v>16.771980280000001</v>
       </c>
       <c r="S5" s="4">
@@ -889,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">B5+1</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2023</v>
       </c>
       <c r="C6" s="4">
@@ -901,7 +919,7 @@
         <v>56.275440500000002</v>
       </c>
       <c r="E6" s="4">
-        <f>C6-D6</f>
+        <f t="shared" si="0"/>
         <v>56.275440500000002</v>
       </c>
       <c r="F6" s="4">
@@ -909,7 +927,7 @@
         <v>28.137720250000001</v>
       </c>
       <c r="G6" s="4">
-        <f>E6-F6</f>
+        <f t="shared" si="1"/>
         <v>28.137720250000001</v>
       </c>
       <c r="H6" s="4">
@@ -917,7 +935,7 @@
         <v>2.2510176200000003</v>
       </c>
       <c r="I6" s="4">
-        <f>G6-H6</f>
+        <f t="shared" si="2"/>
         <v>25.886702630000002</v>
       </c>
       <c r="J6" s="4">
@@ -925,7 +943,7 @@
         <v>6.7530528600000004</v>
       </c>
       <c r="K6" s="4">
-        <f>I6-J6</f>
+        <f t="shared" si="3"/>
         <v>19.133649770000002</v>
       </c>
       <c r="L6" s="4">
@@ -933,7 +951,7 @@
         <v>1.1255088100000001</v>
       </c>
       <c r="M6" s="4">
-        <f>K6-L6</f>
+        <f t="shared" si="4"/>
         <v>18.008140960000002</v>
       </c>
       <c r="N6" s="4">
@@ -941,7 +959,7 @@
         <v>3.7817096016000002</v>
       </c>
       <c r="O6" s="4">
-        <f>M6-N6</f>
+        <f t="shared" si="5"/>
         <v>14.226431358400003</v>
       </c>
       <c r="P6" s="4">
@@ -953,7 +971,7 @@
         <v>0.32781810000000039</v>
       </c>
       <c r="R6" s="4">
-        <f>O6+J6-P6-Q6</f>
+        <f t="shared" si="6"/>
         <v>17.275139688400003</v>
       </c>
       <c r="S6" s="4">
@@ -967,7 +985,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">B6+1</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2024</v>
       </c>
       <c r="C7" s="4">
@@ -979,7 +997,7 @@
         <v>57.963703715000001</v>
       </c>
       <c r="E7" s="4">
-        <f>C7-D7</f>
+        <f t="shared" si="0"/>
         <v>57.963703715000001</v>
       </c>
       <c r="F7" s="4">
@@ -987,7 +1005,7 @@
         <v>28.981851857500001</v>
       </c>
       <c r="G7" s="4">
-        <f>E7-F7</f>
+        <f t="shared" si="1"/>
         <v>28.981851857500001</v>
       </c>
       <c r="H7" s="4">
@@ -995,7 +1013,7 @@
         <v>2.3185481486000001</v>
       </c>
       <c r="I7" s="4">
-        <f>G7-H7</f>
+        <f t="shared" si="2"/>
         <v>26.663303708899999</v>
       </c>
       <c r="J7" s="4">
@@ -1003,7 +1021,7 @@
         <v>6.9556444458000009</v>
       </c>
       <c r="K7" s="4">
-        <f>I7-J7</f>
+        <f t="shared" si="3"/>
         <v>19.707659263099998</v>
       </c>
       <c r="L7" s="4">
@@ -1011,7 +1029,7 @@
         <v>1.1592740743000001</v>
       </c>
       <c r="M7" s="4">
-        <f>K7-L7</f>
+        <f t="shared" si="4"/>
         <v>18.548385188799998</v>
       </c>
       <c r="N7" s="4">
@@ -1019,7 +1037,7 @@
         <v>3.8951608896479994</v>
       </c>
       <c r="O7" s="4">
-        <f>M7-N7</f>
+        <f t="shared" si="5"/>
         <v>14.653224299151997</v>
       </c>
       <c r="P7" s="4">
@@ -1031,7 +1049,7 @@
         <v>0.33765264299999986</v>
       </c>
       <c r="R7" s="4">
-        <f>O7+J7-P7-Q7</f>
+        <f t="shared" si="6"/>
         <v>17.793393879051997</v>
       </c>
       <c r="S7" s="4">
@@ -1045,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <f ca="1">B7+1</f>
+        <f t="shared" ca="1" si="7"/>
         <v>2025</v>
       </c>
       <c r="C8" s="4">
@@ -1057,7 +1075,7 @@
         <v>59.702614826450002</v>
       </c>
       <c r="E8" s="4">
-        <f>C8-D8</f>
+        <f t="shared" si="0"/>
         <v>59.702614826450002</v>
       </c>
       <c r="F8" s="4">
@@ -1065,7 +1083,7 @@
         <v>29.851307413225001</v>
       </c>
       <c r="G8" s="4">
-        <f>E8-F8</f>
+        <f t="shared" si="1"/>
         <v>29.851307413225001</v>
       </c>
       <c r="H8" s="4">
@@ -1073,7 +1091,7 @@
         <v>2.3881045930580003</v>
       </c>
       <c r="I8" s="4">
-        <f>G8-H8</f>
+        <f t="shared" si="2"/>
         <v>27.463202820167002</v>
       </c>
       <c r="J8" s="4">
@@ -1081,7 +1099,7 @@
         <v>7.1643137791740008</v>
       </c>
       <c r="K8" s="4">
-        <f>I8-J8</f>
+        <f t="shared" si="3"/>
         <v>20.298889040993</v>
       </c>
       <c r="L8" s="4">
@@ -1089,7 +1107,7 @@
         <v>1.1940522965290001</v>
       </c>
       <c r="M8" s="4">
-        <f>K8-L8</f>
+        <f t="shared" si="4"/>
         <v>19.104836744463999</v>
       </c>
       <c r="N8" s="4">
@@ -1097,7 +1115,7 @@
         <v>4.0120157163374399</v>
       </c>
       <c r="O8" s="4">
-        <f>M8-N8</f>
+        <f t="shared" si="5"/>
         <v>15.092821028126558</v>
       </c>
       <c r="P8" s="4">
@@ -1109,7 +1127,7 @@
         <v>0.34778222229000022</v>
       </c>
       <c r="R8" s="4">
-        <f>O8+J8-P8-Q8</f>
+        <f t="shared" si="6"/>
         <v>18.327195695423558</v>
       </c>
       <c r="S8" s="4">
@@ -1223,21 +1241,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E4EA94-81AA-9149-9201-4E66100EA077}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6">
         <f ca="1">TODAY()</f>
-        <v>43872</v>
+        <v>43895</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1274,7 +1295,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>0.03</v>
@@ -1282,10 +1303,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1293,25 +1314,25 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4">
-        <f>SUM(DCF!C19:H19)</f>
-        <v>0</v>
+        <f>SUM(DCF!S3:S8)</f>
+        <v>74.712361051937364</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4">
-        <f>DCF!H19*(1+B6)/(B7-B6)</f>
-        <v>0</v>
+        <f>DCF!S8*(1+B6)/(B7-B6)</f>
+        <v>89.128438948062552</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4">
         <v>50</v>
@@ -1319,11 +1340,115 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5">
         <f>B9+B10-B11</f>
-        <v>-50</v>
+        <v>113.84079999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="5">
+        <f>B12/B13</f>
+        <v>11.384079999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86629FFD-1A04-834E-8B20-EACE173174BD}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8">
+        <f>SUM(DCF!S3:S8)</f>
+        <v>74.712361051937364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8">
+        <f>DCF!S8*(1+Assumptions!$B$6)/(Assumptions!$B$7-Assumptions!$B$6)/(1+Assumptions!$B$3)^DCF!$A$8</f>
+        <v>46.290518292930585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8">
+        <f>B2+B3</f>
+        <v>121.00287934486795</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="8">
+        <f>B5-B4</f>
+        <v>119.00287934486795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8">
+        <f>B6/B7</f>
+        <v>11.900287934486794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TEST: Update testing Excel file, don't cover ABC
</commit_message>
<xml_diff>
--- a/autodcf/tests/data/simple_dcf.xlsx
+++ b/autodcf/tests/data/simple_dcf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacklm/Documents/Interests/Programming/Python/autodcf/autodcf/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14122429-D573-2448-9648-1C3253AA0FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58B06C7-E413-824B-AFD6-BF5D0539E613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="2" xr2:uid="{F59C2343-CAF4-9248-9F9B-A15401A49AE8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Year</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Current Share Price</t>
+  </si>
+  <si>
+    <t>absolute_upside_per_share</t>
+  </si>
+  <si>
+    <t>percent_upside_per_share</t>
   </si>
 </sst>
 </file>
@@ -186,12 +195,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -201,11 +211,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1244,7 +1256,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1310,59 +1322,27 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="3"/>
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4">
-        <f>SUM(DCF!S3:S8)</f>
-        <v>74.712361051937364</v>
-      </c>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4">
-        <f>DCF!S8*(1+B6)/(B7-B6)</f>
-        <v>89.128438948062552</v>
-      </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4">
-        <v>50</v>
-      </c>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="5">
-        <f>B9+B10-B11</f>
-        <v>113.84079999999992</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="5">
-        <f>B12/B13</f>
-        <v>11.384079999999992</v>
-      </c>
+      <c r="B14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1371,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86629FFD-1A04-834E-8B20-EACE173174BD}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1451,6 +1431,24 @@
         <v>11.900287934486794</v>
       </c>
     </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B8-Assumptions!B8</f>
+        <v>6.1502879344867942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9">
+        <f>B9/Assumptions!B8</f>
+        <v>1.0696152929542251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>